<commit_message>
DEF:More Dr. W's suggestion, more detail in results for SOA
</commit_message>
<xml_diff>
--- a/DOC/SOA Comparison.xlsx
+++ b/DOC/SOA Comparison.xlsx
@@ -49,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G7" authorId="0">
+    <comment ref="F8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -69,8 +69,38 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-16 vaults
-8 GBps per vault</t>
+ Its not clear whether Neurocube connects ditectly to a vault.
+Looking at the documentation suggests all data goes thru the NoC.
+In which case they assume the DRAM bandwidth can be maintained thru the NoC.
+Did they f%^$%^$^g prove it, I don’t think so.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lee Baker:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Cluster conencts to interconnect network, not directly to a vault
+-&gt; Limited by the interconnect network
+ Its not clear whether Neurocube connects ditectly to a vault.
+Looking at the documentation suggests all data goes thru the NoC.
+</t>
         </r>
       </text>
     </comment>
@@ -79,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="54">
   <si>
     <t>TPU</t>
   </si>
@@ -241,6 +271,9 @@
   </si>
   <si>
     <t>Number of devices to meet bandwidth</t>
+  </si>
+  <si>
+    <t>Area required to meet bandwidth</t>
   </si>
 </sst>
 </file>
@@ -439,7 +472,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="194">
+  <cellStyleXfs count="210">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -634,8 +667,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -794,8 +843,11 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="194">
+  <cellStyles count="210">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -892,6 +944,14 @@
     <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="203" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="205" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="207" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="209" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -988,6 +1048,14 @@
     <cellStyle name="Hyperlink" xfId="188" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="190" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="192" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="194" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="196" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="198" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="202" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="204" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="206" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="208" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Sheet1" xfId="163"/>
   </cellStyles>
@@ -1328,8 +1396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:S55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B15" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1438,8 +1506,8 @@
         <v>128000000000</v>
       </c>
       <c r="G7" s="3">
-        <f>16*8000000000</f>
-        <v>128000000000</v>
+        <f>G8/8</f>
+        <v>32000000000</v>
       </c>
       <c r="H7" s="3">
         <f>4096*606000000/8</f>
@@ -1458,7 +1526,7 @@
       </c>
       <c r="M7" s="14">
         <f>$J$7/G7</f>
-        <v>64</v>
+        <v>256</v>
       </c>
       <c r="N7" s="14">
         <f>$J$7/H7</f>
@@ -1482,8 +1550,8 @@
         <v>1024000000000</v>
       </c>
       <c r="G8" s="2">
-        <f>G7*8</f>
-        <v>1024000000000</v>
+        <f>256000000000</f>
+        <v>256000000000</v>
       </c>
       <c r="H8" s="3">
         <f>H7*8</f>
@@ -1569,7 +1637,7 @@
       </c>
       <c r="G12" s="9">
         <f>$E$2/G8</f>
-        <v>32.2265625</v>
+        <v>128.90625</v>
       </c>
       <c r="H12" s="9">
         <f>$E$2/H8</f>
@@ -1596,9 +1664,12 @@
       </c>
       <c r="G13" s="45">
         <f>G12*G9</f>
-        <v>354.4921875</v>
-      </c>
-      <c r="H13" s="45"/>
+        <v>1417.96875</v>
+      </c>
+      <c r="H13" s="45">
+        <f>H12*H9</f>
+        <v>212.31774056311883</v>
+      </c>
       <c r="I13" s="45">
         <v>250</v>
       </c>
@@ -1648,7 +1719,7 @@
         <v>68</v>
       </c>
       <c r="G16" s="2">
-        <v>68</v>
+        <v>99</v>
       </c>
       <c r="H16" s="9">
         <v>67</v>
@@ -1665,7 +1736,7 @@
       </c>
       <c r="M16" s="15">
         <f>$J$16/G16</f>
-        <v>5.1470588235294121</v>
+        <v>3.5353535353535355</v>
       </c>
       <c r="N16" s="15">
         <f>$J$16/H16</f>
@@ -1692,15 +1763,30 @@
       <c r="D19" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
+      <c r="E19" s="9">
+        <f>((E13/(E12*E16))*1000)*(1000000000/E10)</f>
+        <v>190.47619047619048</v>
+      </c>
+      <c r="F19" s="9">
+        <f>((F13/(F12*F16))*1000)*(1000000000/F10)</f>
+        <v>204.11764705882354</v>
+      </c>
       <c r="G19" s="9">
-        <f>G18*1000/G17</f>
-        <v>304.87804878048786</v>
-      </c>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
+        <f>((G13/(G12*G16))*1000)*(1000000000/G10)</f>
+        <v>111.1111111111111</v>
+      </c>
+      <c r="H19" s="9">
+        <f>((H13/(H12*H16))*1000)*(1000000000/H10)</f>
+        <v>393.33037781390078</v>
+      </c>
+      <c r="I19" s="9">
+        <f>((I13/(I12*I16))*1000)*(1000000000/I10)</f>
+        <v>59.833214913428826</v>
+      </c>
+      <c r="J19" s="9">
+        <f>((J13/J16)*1000)*(1000000000/J10)</f>
+        <v>428.57142857142856</v>
+      </c>
       <c r="L19" s="55" t="s">
         <v>34</v>
       </c>
@@ -1841,7 +1927,7 @@
       </c>
       <c r="G24" s="9">
         <f t="shared" si="1"/>
-        <v>544</v>
+        <v>792</v>
       </c>
       <c r="H24" s="9">
         <f t="shared" si="1"/>
@@ -1861,6 +1947,31 @@
       </c>
     </row>
     <row r="25" spans="4:19">
+      <c r="D25" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" s="9">
+        <f>E12*E16</f>
+        <v>34375</v>
+      </c>
+      <c r="F25" s="9">
+        <f>F12*F16</f>
+        <v>2191.40625</v>
+      </c>
+      <c r="G25" s="9">
+        <f>G12*G16</f>
+        <v>12761.71875</v>
+      </c>
+      <c r="H25" s="9">
+        <f>H12*H16</f>
+        <v>890.75069616336634</v>
+      </c>
+      <c r="I25" s="56">
+        <v>34375</v>
+      </c>
+      <c r="J25" s="56">
+        <v>34375</v>
+      </c>
       <c r="P25">
         <v>64</v>
       </c>
@@ -1891,7 +2002,7 @@
       </c>
       <c r="G27" s="4">
         <f t="shared" si="2"/>
-        <v>7.8125E-3</v>
+        <v>3.125E-2</v>
       </c>
       <c r="H27" s="4">
         <f t="shared" si="2"/>
@@ -1956,7 +2067,7 @@
       </c>
       <c r="G31" s="18">
         <f t="shared" si="3"/>
-        <v>128</v>
+        <v>32</v>
       </c>
       <c r="H31" s="18">
         <f t="shared" si="3"/>
@@ -2069,7 +2180,7 @@
       </c>
       <c r="G36" s="21">
         <f>$E$2/G8*G9</f>
-        <v>354.4921875</v>
+        <v>1417.96875</v>
       </c>
       <c r="H36" s="21">
         <f>$E$2/H8*H9</f>
@@ -2094,7 +2205,7 @@
       </c>
       <c r="G37" s="22">
         <f>G36/$J$13</f>
-        <v>4.7265625</v>
+        <v>18.90625</v>
       </c>
       <c r="H37" s="22">
         <f>H36/$J$13</f>
@@ -2123,7 +2234,7 @@
       </c>
       <c r="G38" s="42">
         <f>MAX(G34,G36)</f>
-        <v>354.4921875</v>
+        <v>1417.96875</v>
       </c>
       <c r="H38" s="42">
         <f>MAX(H34,H36)</f>
@@ -2150,7 +2261,7 @@
       </c>
       <c r="G39" s="44">
         <f>G38/$J$13</f>
-        <v>4.7265625</v>
+        <v>18.90625</v>
       </c>
       <c r="H39" s="44">
         <f>H38/$J$13</f>
@@ -2177,7 +2288,7 @@
       </c>
       <c r="G40" s="21">
         <f>MAX(G23,G12)*G16</f>
-        <v>2191.40625</v>
+        <v>12761.71875</v>
       </c>
       <c r="H40" s="21">
         <f>MAX(H23,H12)*H16</f>
@@ -2202,7 +2313,7 @@
       </c>
       <c r="G41" s="22">
         <f>G40/$J$16</f>
-        <v>6.2611607142857144</v>
+        <v>36.462053571428569</v>
       </c>
       <c r="H41" s="22">
         <f>H40/$J$16</f>
@@ -2288,7 +2399,7 @@
       </c>
       <c r="G49" s="32">
         <f t="shared" si="4"/>
-        <v>0.24824242424242424</v>
+        <v>6.2060606060606059E-2</v>
       </c>
       <c r="H49" s="32">
         <f t="shared" si="4"/>
@@ -2357,7 +2468,7 @@
       </c>
       <c r="G54" s="32">
         <f t="shared" si="5"/>
-        <v>4.0283203125</v>
+        <v>16.11328125</v>
       </c>
       <c r="H54" s="32">
         <f t="shared" si="5"/>

</xml_diff>